<commit_message>
First DoE ML commit
</commit_message>
<xml_diff>
--- a/Results/Errors/LinearSVM_samples_error.xlsx
+++ b/Results/Errors/LinearSVM_samples_error.xlsx
@@ -475,7 +475,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="n">
-        <v>0.11494</v>
+        <v>0.11073</v>
       </c>
       <c r="C2" t="n">
         <v>18</v>
@@ -501,7 +501,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="n">
-        <v>0.31437</v>
+        <v>0.30114</v>
       </c>
       <c r="C3" t="n">
         <v>24</v>
@@ -527,7 +527,7 @@
         <v>80</v>
       </c>
       <c r="B4" t="n">
-        <v>0.31442</v>
+        <v>0.3012</v>
       </c>
       <c r="C4" t="n">
         <v>22</v>
@@ -553,7 +553,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>0.31453</v>
+        <v>0.3013</v>
       </c>
       <c r="C5" t="n">
         <v>18</v>
@@ -579,7 +579,7 @@
         <v>93</v>
       </c>
       <c r="B6" t="n">
-        <v>0.31453</v>
+        <v>0.3013</v>
       </c>
       <c r="C6" t="n">
         <v>18</v>
@@ -605,7 +605,7 @@
         <v>73</v>
       </c>
       <c r="B7" t="n">
-        <v>0.31453</v>
+        <v>0.3013</v>
       </c>
       <c r="C7" t="n">
         <v>18</v>
@@ -631,7 +631,7 @@
         <v>75</v>
       </c>
       <c r="B8" t="n">
-        <v>0.31458</v>
+        <v>0.30136</v>
       </c>
       <c r="C8" t="n">
         <v>16</v>
@@ -657,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>0.31458</v>
+        <v>0.30136</v>
       </c>
       <c r="C9" t="n">
         <v>16</v>
@@ -683,7 +683,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="n">
-        <v>0.31464</v>
+        <v>0.30141</v>
       </c>
       <c r="C10" t="n">
         <v>14</v>
@@ -709,7 +709,7 @@
         <v>70</v>
       </c>
       <c r="B11" t="n">
-        <v>0.31464</v>
+        <v>0.30141</v>
       </c>
       <c r="C11" t="n">
         <v>14</v>
@@ -735,7 +735,7 @@
         <v>89</v>
       </c>
       <c r="B12" t="n">
-        <v>0.31467</v>
+        <v>0.30144</v>
       </c>
       <c r="C12" t="n">
         <v>18</v>
@@ -761,7 +761,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="n">
-        <v>0.31475</v>
+        <v>0.30152</v>
       </c>
       <c r="C13" t="n">
         <v>10</v>
@@ -787,7 +787,7 @@
         <v>83</v>
       </c>
       <c r="B14" t="n">
-        <v>0.31488</v>
+        <v>0.30166</v>
       </c>
       <c r="C14" t="n">
         <v>10</v>
@@ -813,7 +813,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>1.14231</v>
+        <v>1.17183</v>
       </c>
       <c r="C15" t="n">
         <v>16</v>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="n">
-        <v>1.14258</v>
+        <v>1.17212</v>
       </c>
       <c r="C16" t="n">
         <v>20</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>1.14362</v>
+        <v>1.17319</v>
       </c>
       <c r="C17" t="n">
         <v>30</v>
@@ -891,7 +891,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>1.30983</v>
+        <v>1.34651</v>
       </c>
       <c r="C18" t="n">
         <v>18</v>
@@ -917,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="n">
-        <v>2.06805</v>
+        <v>2.09828</v>
       </c>
       <c r="C19" t="n">
         <v>30</v>
@@ -943,7 +943,7 @@
         <v>33</v>
       </c>
       <c r="B20" t="n">
-        <v>2.21991</v>
+        <v>2.25518</v>
       </c>
       <c r="C20" t="n">
         <v>22</v>
@@ -969,7 +969,7 @@
         <v>31</v>
       </c>
       <c r="B21" t="n">
-        <v>2.22027</v>
+        <v>2.25555</v>
       </c>
       <c r="C21" t="n">
         <v>18</v>
@@ -995,7 +995,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="n">
-        <v>2.22027</v>
+        <v>2.25555</v>
       </c>
       <c r="C22" t="n">
         <v>18</v>
@@ -1021,7 +1021,7 @@
         <v>47</v>
       </c>
       <c r="B23" t="n">
-        <v>2.22062</v>
+        <v>2.25592</v>
       </c>
       <c r="C23" t="n">
         <v>14</v>
@@ -1047,7 +1047,7 @@
         <v>64</v>
       </c>
       <c r="B24" t="n">
-        <v>2.22072</v>
+        <v>2.25602</v>
       </c>
       <c r="C24" t="n">
         <v>18</v>
@@ -1073,7 +1073,7 @@
         <v>62</v>
       </c>
       <c r="B25" t="n">
-        <v>2.22108</v>
+        <v>2.25639</v>
       </c>
       <c r="C25" t="n">
         <v>14</v>
@@ -1099,7 +1099,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="n">
-        <v>2.22108</v>
+        <v>2.25639</v>
       </c>
       <c r="C26" t="n">
         <v>14</v>
@@ -1125,7 +1125,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="n">
-        <v>2.43381</v>
+        <v>2.47615</v>
       </c>
       <c r="C27" t="n">
         <v>22</v>
@@ -1151,7 +1151,7 @@
         <v>39</v>
       </c>
       <c r="B28" t="n">
-        <v>4.68899</v>
+        <v>4.80288</v>
       </c>
       <c r="C28" t="n">
         <v>24</v>
@@ -1177,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="n">
-        <v>4.68919</v>
+        <v>4.80309</v>
       </c>
       <c r="C29" t="n">
         <v>22</v>
@@ -1203,7 +1203,7 @@
         <v>68</v>
       </c>
       <c r="B30" t="n">
-        <v>4.6903</v>
+        <v>4.80424</v>
       </c>
       <c r="C30" t="n">
         <v>16</v>
@@ -1229,7 +1229,7 @@
         <v>65</v>
       </c>
       <c r="B31" t="n">
-        <v>4.6909</v>
+        <v>4.80486</v>
       </c>
       <c r="C31" t="n">
         <v>10</v>

</xml_diff>